<commit_message>
update the daf in IPHRA to use the right colum
</commit_message>
<xml_diff>
--- a/inst/iphra_analysis/resources/daf.xlsx
+++ b/inst/iphra_analysis/resources/daf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abraham.azar\Desktop\git\IPHRA_toolkit\analysis\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abraham.azar\Desktop\git\impactR4PHU\inst\iphra_analysis\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBA038F-E1D4-4DF3-8A03-D266070D4D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7239FD-FDA2-4414-B8DA-38C2EAF9A962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="6" r:id="rId1"/>
@@ -191,9 +191,6 @@
     <t>Individual Sex</t>
   </si>
   <si>
-    <t>ind_age_years</t>
-  </si>
-  <si>
     <t>Individual Age in Years</t>
   </si>
   <si>
@@ -933,6 +930,9 @@
   </si>
   <si>
     <t>fsl_num_meals</t>
+  </si>
+  <si>
+    <t>calc_final_age_years</t>
   </si>
 </sst>
 </file>
@@ -1585,8 +1585,8 @@
   <dimension ref="A1:G148"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C148" sqref="C148"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1971,10 +1971,10 @@
         <v>46</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
@@ -1990,10 +1990,10 @@
         <v>46</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
@@ -2009,10 +2009,10 @@
         <v>46</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
@@ -2028,10 +2028,10 @@
         <v>29</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
@@ -2047,10 +2047,10 @@
         <v>29</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
@@ -2066,10 +2066,10 @@
         <v>29</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
@@ -2085,10 +2085,10 @@
         <v>29</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
@@ -2104,10 +2104,10 @@
         <v>29</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
@@ -2123,10 +2123,10 @@
         <v>29</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
@@ -2142,10 +2142,10 @@
         <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
@@ -2158,13 +2158,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
@@ -2177,13 +2177,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
@@ -2193,18 +2193,18 @@
         <v>11</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
@@ -2219,13 +2219,13 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="s">
@@ -2235,22 +2235,22 @@
         <v>11</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>11</v>
@@ -2259,13 +2259,13 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
@@ -2278,13 +2278,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
@@ -2297,13 +2297,13 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1" t="s">
@@ -2313,18 +2313,18 @@
         <v>11</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1" t="s">
@@ -2339,13 +2339,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1" t="s">
@@ -2355,22 +2355,22 @@
         <v>11</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>11</v>
@@ -2379,13 +2379,13 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1" t="s">
@@ -2398,13 +2398,13 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1" t="s">
@@ -2414,18 +2414,18 @@
         <v>11</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1" t="s">
@@ -2435,18 +2435,18 @@
         <v>11</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1" t="s">
@@ -2459,13 +2459,13 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1" t="s">
@@ -2475,18 +2475,18 @@
         <v>11</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1" t="s">
@@ -2496,18 +2496,18 @@
         <v>11</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1" t="s">
@@ -2520,13 +2520,13 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1" t="s">
@@ -2536,18 +2536,18 @@
         <v>11</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1" t="s">
@@ -2557,22 +2557,22 @@
         <v>11</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>11</v>
@@ -2581,38 +2581,38 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>11</v>
@@ -2623,13 +2623,13 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1" t="s">
@@ -2642,13 +2642,13 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1" t="s">
@@ -2663,13 +2663,13 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1" t="s">
@@ -2682,13 +2682,13 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1" t="s">
@@ -2701,13 +2701,13 @@
     </row>
     <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1" t="s">
@@ -2720,17 +2720,17 @@
     </row>
     <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>11</v>
@@ -2739,17 +2739,17 @@
     </row>
     <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>11</v>
@@ -2758,17 +2758,17 @@
     </row>
     <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>11</v>
@@ -2777,17 +2777,17 @@
     </row>
     <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>11</v>
@@ -2796,13 +2796,13 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1" t="s">
@@ -2815,13 +2815,13 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="1" t="s">
@@ -2834,13 +2834,13 @@
     </row>
     <row r="64" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1" t="s">
@@ -2853,13 +2853,13 @@
     </row>
     <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1" t="s">
@@ -2872,13 +2872,13 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1" t="s">
@@ -2891,13 +2891,13 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1" t="s">
@@ -2910,13 +2910,13 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1" t="s">
@@ -2929,13 +2929,13 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="1" t="s">
@@ -2948,13 +2948,13 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="1" t="s">
@@ -2967,13 +2967,13 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1" t="s">
@@ -2986,13 +2986,13 @@
     </row>
     <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1" t="s">
@@ -3005,13 +3005,13 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="1" t="s">
@@ -3024,13 +3024,13 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1" t="s">
@@ -3043,13 +3043,13 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B75" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C75" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E75" t="s">
         <v>10</v>
@@ -3060,13 +3060,13 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B76" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C76" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E76" t="s">
         <v>10</v>
@@ -3077,13 +3077,13 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B77" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C77" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E77" t="s">
         <v>10</v>
@@ -3094,13 +3094,13 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B78" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C78" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E78" t="s">
         <v>10</v>
@@ -3111,13 +3111,13 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B79" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C79" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E79" t="s">
         <v>10</v>
@@ -3128,13 +3128,13 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B80" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C80" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E80" t="s">
         <v>10</v>
@@ -3145,13 +3145,13 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B81" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C81" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E81" t="s">
         <v>10</v>
@@ -3162,13 +3162,13 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B82" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C82" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E82" t="s">
         <v>10</v>
@@ -3179,13 +3179,13 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B83" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C83" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E83" t="s">
         <v>10</v>
@@ -3196,13 +3196,13 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B84" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C84" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E84" t="s">
         <v>24</v>
@@ -3213,13 +3213,13 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>116</v>
+      </c>
+      <c r="B85" t="s">
         <v>117</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" t="s">
         <v>118</v>
-      </c>
-      <c r="C85" t="s">
-        <v>119</v>
       </c>
       <c r="E85" t="s">
         <v>10</v>
@@ -3230,13 +3230,13 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B86" t="s">
+        <v>119</v>
+      </c>
+      <c r="C86" t="s">
         <v>120</v>
-      </c>
-      <c r="C86" t="s">
-        <v>121</v>
       </c>
       <c r="E86" t="s">
         <v>10</v>
@@ -3247,13 +3247,13 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B87" t="s">
+        <v>121</v>
+      </c>
+      <c r="C87" t="s">
         <v>122</v>
-      </c>
-      <c r="C87" t="s">
-        <v>123</v>
       </c>
       <c r="E87" t="s">
         <v>24</v>
@@ -3264,13 +3264,13 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B88" t="s">
+        <v>123</v>
+      </c>
+      <c r="C88" t="s">
         <v>124</v>
-      </c>
-      <c r="C88" t="s">
-        <v>125</v>
       </c>
       <c r="E88" t="s">
         <v>24</v>
@@ -3281,13 +3281,13 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B89" t="s">
+        <v>125</v>
+      </c>
+      <c r="C89" t="s">
         <v>126</v>
-      </c>
-      <c r="C89" t="s">
-        <v>127</v>
       </c>
       <c r="E89" t="s">
         <v>10</v>
@@ -3298,13 +3298,13 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B90" t="s">
+        <v>127</v>
+      </c>
+      <c r="C90" t="s">
         <v>128</v>
-      </c>
-      <c r="C90" t="s">
-        <v>129</v>
       </c>
       <c r="E90" t="s">
         <v>24</v>
@@ -3315,13 +3315,13 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B91" t="s">
+        <v>129</v>
+      </c>
+      <c r="C91" t="s">
         <v>130</v>
-      </c>
-      <c r="C91" t="s">
-        <v>131</v>
       </c>
       <c r="E91" t="s">
         <v>10</v>
@@ -3332,16 +3332,16 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B92" t="s">
+        <v>131</v>
+      </c>
+      <c r="C92" t="s">
         <v>132</v>
       </c>
-      <c r="C92" t="s">
-        <v>133</v>
-      </c>
       <c r="E92" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F92" t="s">
         <v>11</v>
@@ -3349,13 +3349,13 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B93" t="s">
+        <v>133</v>
+      </c>
+      <c r="C93" t="s">
         <v>134</v>
-      </c>
-      <c r="C93" t="s">
-        <v>135</v>
       </c>
       <c r="E93" t="s">
         <v>10</v>
@@ -3366,16 +3366,16 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B94" t="s">
+        <v>135</v>
+      </c>
+      <c r="C94" t="s">
         <v>136</v>
       </c>
-      <c r="C94" t="s">
-        <v>137</v>
-      </c>
       <c r="E94" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F94" t="s">
         <v>11</v>
@@ -3383,13 +3383,13 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B95" t="s">
+        <v>137</v>
+      </c>
+      <c r="C95" t="s">
         <v>138</v>
-      </c>
-      <c r="C95" t="s">
-        <v>139</v>
       </c>
       <c r="E95" t="s">
         <v>10</v>
@@ -3400,16 +3400,16 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B96" t="s">
+        <v>139</v>
+      </c>
+      <c r="C96" t="s">
         <v>140</v>
       </c>
-      <c r="C96" t="s">
-        <v>141</v>
-      </c>
       <c r="E96" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F96" t="s">
         <v>11</v>
@@ -3417,13 +3417,13 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B97" t="s">
+        <v>141</v>
+      </c>
+      <c r="C97" t="s">
         <v>142</v>
-      </c>
-      <c r="C97" t="s">
-        <v>143</v>
       </c>
       <c r="E97" t="s">
         <v>10</v>
@@ -3434,16 +3434,16 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B98" t="s">
+        <v>143</v>
+      </c>
+      <c r="C98" t="s">
         <v>144</v>
       </c>
-      <c r="C98" t="s">
-        <v>145</v>
-      </c>
       <c r="E98" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F98" t="s">
         <v>11</v>
@@ -3451,13 +3451,13 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B99" t="s">
+        <v>145</v>
+      </c>
+      <c r="C99" t="s">
         <v>146</v>
-      </c>
-      <c r="C99" t="s">
-        <v>147</v>
       </c>
       <c r="E99" t="s">
         <v>10</v>
@@ -3468,16 +3468,16 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B100" t="s">
+        <v>147</v>
+      </c>
+      <c r="C100" t="s">
         <v>148</v>
       </c>
-      <c r="C100" t="s">
-        <v>149</v>
-      </c>
       <c r="E100" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F100" t="s">
         <v>11</v>
@@ -3485,13 +3485,13 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B101" t="s">
+        <v>149</v>
+      </c>
+      <c r="C101" t="s">
         <v>150</v>
-      </c>
-      <c r="C101" t="s">
-        <v>151</v>
       </c>
       <c r="E101" t="s">
         <v>10</v>
@@ -3502,16 +3502,16 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B102" t="s">
+        <v>151</v>
+      </c>
+      <c r="C102" t="s">
         <v>152</v>
       </c>
-      <c r="C102" t="s">
-        <v>153</v>
-      </c>
       <c r="E102" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F102" t="s">
         <v>11</v>
@@ -3519,13 +3519,13 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>153</v>
+      </c>
+      <c r="B103" t="s">
+        <v>275</v>
+      </c>
+      <c r="C103" t="s">
         <v>154</v>
-      </c>
-      <c r="B103" t="s">
-        <v>276</v>
-      </c>
-      <c r="C103" t="s">
-        <v>155</v>
       </c>
       <c r="E103" t="s">
         <v>10</v>
@@ -3536,13 +3536,13 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B104" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C104" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E104" t="s">
         <v>24</v>
@@ -3553,13 +3553,13 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B105" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C105" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E105" t="s">
         <v>24</v>
@@ -3568,18 +3568,18 @@
         <v>11</v>
       </c>
       <c r="G105" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B106" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C106" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E106" t="s">
         <v>24</v>
@@ -3588,18 +3588,18 @@
         <v>11</v>
       </c>
       <c r="G106" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B107" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C107" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E107" t="s">
         <v>10</v>
@@ -3610,13 +3610,13 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B108" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C108" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E108" t="s">
         <v>10</v>
@@ -3627,13 +3627,13 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B109" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C109" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E109" t="s">
         <v>10</v>
@@ -3644,13 +3644,13 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B110" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C110" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E110" t="s">
         <v>10</v>
@@ -3659,18 +3659,18 @@
         <v>11</v>
       </c>
       <c r="G110" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B111" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C111" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E111" t="s">
         <v>10</v>
@@ -3679,18 +3679,18 @@
         <v>11</v>
       </c>
       <c r="G111" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B112" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C112" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E112" t="s">
         <v>10</v>
@@ -3701,13 +3701,13 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B113" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C113" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E113" t="s">
         <v>10</v>
@@ -3718,13 +3718,13 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B114" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C114" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E114" t="s">
         <v>10</v>
@@ -3733,21 +3733,21 @@
         <v>11</v>
       </c>
       <c r="G114" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B115" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C115" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E115" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F115" t="s">
         <v>11</v>
@@ -3755,16 +3755,16 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B116" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C116" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E116" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F116" t="s">
         <v>11</v>
@@ -3772,36 +3772,36 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B117" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C117" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E117" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F117" t="s">
         <v>11</v>
       </c>
       <c r="G117" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B118" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C118" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E118" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F118" t="s">
         <v>11</v>
@@ -3809,33 +3809,33 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B119" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C119" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E119" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F119" t="s">
         <v>11</v>
       </c>
       <c r="G119" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B120" t="s">
+        <v>163</v>
+      </c>
+      <c r="C120" t="s">
         <v>164</v>
-      </c>
-      <c r="C120" t="s">
-        <v>165</v>
       </c>
       <c r="E120" t="s">
         <v>10</v>
@@ -3846,13 +3846,13 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
+        <v>165</v>
+      </c>
+      <c r="B121" t="s">
         <v>166</v>
       </c>
-      <c r="B121" t="s">
+      <c r="C121" t="s">
         <v>167</v>
-      </c>
-      <c r="C121" t="s">
-        <v>168</v>
       </c>
       <c r="E121" t="s">
         <v>10</v>
@@ -3863,13 +3863,13 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B122" t="s">
+        <v>168</v>
+      </c>
+      <c r="C122" t="s">
         <v>169</v>
-      </c>
-      <c r="C122" t="s">
-        <v>170</v>
       </c>
       <c r="E122" t="s">
         <v>24</v>
@@ -3880,13 +3880,13 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B123" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C123" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E123" t="s">
         <v>24</v>
@@ -3895,18 +3895,18 @@
         <v>11</v>
       </c>
       <c r="G123" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B124" t="s">
+        <v>170</v>
+      </c>
+      <c r="C124" t="s">
         <v>171</v>
-      </c>
-      <c r="C124" t="s">
-        <v>172</v>
       </c>
       <c r="E124" t="s">
         <v>10</v>
@@ -3917,13 +3917,13 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B125" t="s">
+        <v>172</v>
+      </c>
+      <c r="C125" t="s">
         <v>173</v>
-      </c>
-      <c r="C125" t="s">
-        <v>174</v>
       </c>
       <c r="E125" t="s">
         <v>10</v>
@@ -3934,13 +3934,13 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B126" t="s">
+        <v>174</v>
+      </c>
+      <c r="C126" t="s">
         <v>175</v>
-      </c>
-      <c r="C126" t="s">
-        <v>176</v>
       </c>
       <c r="E126" t="s">
         <v>10</v>
@@ -3951,13 +3951,13 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B127" t="s">
+        <v>176</v>
+      </c>
+      <c r="C127" t="s">
         <v>177</v>
-      </c>
-      <c r="C127" t="s">
-        <v>178</v>
       </c>
       <c r="E127" t="s">
         <v>10</v>
@@ -3968,13 +3968,13 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B128" t="s">
+        <v>178</v>
+      </c>
+      <c r="C128" t="s">
         <v>179</v>
-      </c>
-      <c r="C128" t="s">
-        <v>180</v>
       </c>
       <c r="E128" t="s">
         <v>24</v>
@@ -3985,13 +3985,13 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B129" t="s">
+        <v>180</v>
+      </c>
+      <c r="C129" t="s">
         <v>181</v>
-      </c>
-      <c r="C129" t="s">
-        <v>182</v>
       </c>
       <c r="E129" t="s">
         <v>10</v>
@@ -4002,13 +4002,13 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B130" t="s">
+        <v>182</v>
+      </c>
+      <c r="C130" t="s">
         <v>183</v>
-      </c>
-      <c r="C130" t="s">
-        <v>184</v>
       </c>
       <c r="E130" t="s">
         <v>24</v>
@@ -4019,13 +4019,13 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B131" t="s">
+        <v>184</v>
+      </c>
+      <c r="C131" t="s">
         <v>185</v>
-      </c>
-      <c r="C131" t="s">
-        <v>186</v>
       </c>
       <c r="E131" t="s">
         <v>10</v>
@@ -4036,13 +4036,13 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B132" t="s">
+        <v>186</v>
+      </c>
+      <c r="C132" t="s">
         <v>187</v>
-      </c>
-      <c r="C132" t="s">
-        <v>188</v>
       </c>
       <c r="E132" t="s">
         <v>10</v>
@@ -4053,13 +4053,13 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B133" t="s">
+        <v>188</v>
+      </c>
+      <c r="C133" t="s">
         <v>189</v>
-      </c>
-      <c r="C133" t="s">
-        <v>190</v>
       </c>
       <c r="E133" t="s">
         <v>10</v>
@@ -4070,13 +4070,13 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B134" t="s">
+        <v>190</v>
+      </c>
+      <c r="C134" t="s">
         <v>191</v>
-      </c>
-      <c r="C134" t="s">
-        <v>192</v>
       </c>
       <c r="E134" t="s">
         <v>10</v>
@@ -4087,13 +4087,13 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B135" t="s">
+        <v>192</v>
+      </c>
+      <c r="C135" t="s">
         <v>193</v>
-      </c>
-      <c r="C135" t="s">
-        <v>194</v>
       </c>
       <c r="E135" t="s">
         <v>10</v>
@@ -4104,13 +4104,13 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B136" t="s">
+        <v>194</v>
+      </c>
+      <c r="C136" t="s">
         <v>195</v>
-      </c>
-      <c r="C136" t="s">
-        <v>196</v>
       </c>
       <c r="E136" t="s">
         <v>10</v>
@@ -4121,13 +4121,13 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B137" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C137" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E137" t="s">
         <v>10</v>
@@ -4138,13 +4138,13 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B138" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C138" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E138" t="s">
         <v>10</v>
@@ -4155,13 +4155,13 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B139" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C139" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E139" t="s">
         <v>10</v>
@@ -4172,16 +4172,16 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B140" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C140" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E140" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F140" t="s">
         <v>11</v>
@@ -4189,13 +4189,13 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B141" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C141" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E141" t="s">
         <v>10</v>
@@ -4206,13 +4206,13 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B142" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C142" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E142" t="s">
         <v>10</v>
@@ -4223,13 +4223,13 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B143" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C143" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E143" t="s">
         <v>24</v>
@@ -4240,13 +4240,13 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B144" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C144" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E144" t="s">
         <v>10</v>
@@ -4257,13 +4257,13 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B145" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C145" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E145" t="s">
         <v>10</v>
@@ -4274,13 +4274,13 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B146" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C146" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E146" t="s">
         <v>10</v>
@@ -4291,13 +4291,13 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B147" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C147" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E147" t="s">
         <v>10</v>
@@ -4308,16 +4308,16 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B148" t="s">
+        <v>92</v>
+      </c>
+      <c r="C148" t="s">
         <v>93</v>
       </c>
-      <c r="C148" t="s">
-        <v>94</v>
-      </c>
       <c r="E148" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F148" t="s">
         <v>11</v>
@@ -4326,55 +4326,35 @@
   </sheetData>
   <autoFilter ref="A1:G136" xr:uid="{CF08D581-7D6B-4201-8B78-772150F80729}"/>
   <phoneticPr fontId="5" type="noConversion"/>
+  <conditionalFormatting sqref="B57">
+    <cfRule type="duplicateValues" dxfId="7" priority="33"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B58">
+    <cfRule type="duplicateValues" dxfId="6" priority="34"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B59">
+    <cfRule type="duplicateValues" dxfId="5" priority="35"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B60">
-    <cfRule type="duplicateValues" dxfId="7" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B61">
-    <cfRule type="duplicateValues" dxfId="6" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64">
-    <cfRule type="duplicateValues" dxfId="5" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B65">
-    <cfRule type="duplicateValues" dxfId="4" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B72">
-    <cfRule type="duplicateValues" dxfId="3" priority="32"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B57">
-    <cfRule type="duplicateValues" dxfId="2" priority="33"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B58">
-    <cfRule type="duplicateValues" dxfId="1" priority="34"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B59">
-    <cfRule type="duplicateValues" dxfId="0" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="32"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e7a156ab-dec1-49fa-a9cf-4ddad9eb4e7c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7a5b9cf8-6f84-47d8-bb23-7f0863df71c6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100873D3DDBB405ED4AA6367858D626971E" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="480f6128cb4bbd073f6326125a41424c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7a5b9cf8-6f84-47d8-bb23-7f0863df71c6" xmlns:ns3="e7a156ab-dec1-49fa-a9cf-4ddad9eb4e7c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="379a74a9217f9861f5630dd08d9dc250" ns2:_="" ns3:_="">
     <xsd:import namespace="7a5b9cf8-6f84-47d8-bb23-7f0863df71c6"/>
@@ -4603,26 +4583,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89BA09EB-57CB-4666-A146-B7C07ECE43F8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e7a156ab-dec1-49fa-a9cf-4ddad9eb4e7c"/>
-    <ds:schemaRef ds:uri="7a5b9cf8-6f84-47d8-bb23-7f0863df71c6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E327905-A0EA-4A05-B28C-1D29BC6AA07D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e7a156ab-dec1-49fa-a9cf-4ddad9eb4e7c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7a5b9cf8-6f84-47d8-bb23-7f0863df71c6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FC56506-C652-4BC8-B530-606F47E08B8E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4639,4 +4620,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E327905-A0EA-4A05-B28C-1D29BC6AA07D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89BA09EB-57CB-4666-A146-B7C07ECE43F8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e7a156ab-dec1-49fa-a9cf-4ddad9eb4e7c"/>
+    <ds:schemaRef ds:uri="7a5b9cf8-6f84-47d8-bb23-7f0863df71c6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>